<commit_message>
forms generation corrected. NCL Library added. Diall scheduller corrected.
</commit_message>
<xml_diff>
--- a/forms/gnhsRegularDynamicVacationForm.xlsx
+++ b/forms/gnhsRegularDynamicVacationForm.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28615"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10611"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/murad/Projects/chatbot/chatbot/forms/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/booogie-man-07/IdeaProjects/chatbot/forms/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4210807B-6C8A-6245-87A7-744BAD8A3EA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -126,8 +127,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="6">
     <font>
       <sz val="8"/>
       <color rgb="FF000000"/>
@@ -135,40 +136,9 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
       <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
     </font>
     <font>
       <u/>
@@ -183,6 +153,19 @@
       <color theme="11"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="GothamPro-Medium"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="GothamPro-Medium"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="2">
@@ -222,106 +205,89 @@
   </borders>
   <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -336,6 +302,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -603,339 +572,480 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr enableFormatConditionsCalculation="0">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A5:E51"/>
+  <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.25" defaultRowHeight="11.5" customHeight="1" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.25" defaultRowHeight="11.5" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="7.25" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.5" style="4" customWidth="1"/>
-    <col min="3" max="3" width="36.25" style="4" customWidth="1"/>
-    <col min="4" max="4" width="10.25" style="4" customWidth="1"/>
-    <col min="5" max="5" width="77.5" style="4" customWidth="1"/>
+    <col min="2" max="2" width="19.5" style="2" customWidth="1"/>
+    <col min="3" max="3" width="36.25" style="2" customWidth="1"/>
+    <col min="4" max="4" width="10.25" style="2" customWidth="1"/>
+    <col min="5" max="5" width="77.5" style="2" customWidth="1"/>
     <col min="6" max="16384" width="10.25" style="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="4:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D5" s="20" t="s">
+    <row r="1" spans="1:5" ht="11.5" customHeight="1">
+      <c r="A1" s="7"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+    </row>
+    <row r="2" spans="1:5" ht="11.5" customHeight="1">
+      <c r="A2" s="7"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+    </row>
+    <row r="3" spans="1:5" ht="11.5" customHeight="1">
+      <c r="A3" s="7"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+    </row>
+    <row r="4" spans="1:5" ht="11.5" customHeight="1">
+      <c r="A4" s="7"/>
+      <c r="B4" s="8"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
+    </row>
+    <row r="5" spans="1:5" ht="19" customHeight="1">
+      <c r="A5" s="7"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="20"/>
-    </row>
-    <row r="6" spans="4:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D6" s="20"/>
-      <c r="E6" s="20"/>
-    </row>
-    <row r="7" spans="4:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D7" s="2" t="s">
+      <c r="E5" s="9"/>
+    </row>
+    <row r="6" spans="1:5" ht="19" customHeight="1">
+      <c r="A6" s="7"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+    </row>
+    <row r="7" spans="1:5" ht="19" customHeight="1">
+      <c r="A7" s="7"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="11" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="4:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="E8" s="5" t="s">
+    <row r="8" spans="1:5" ht="14">
+      <c r="A8" s="7"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="4:5" ht="5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-    </row>
-    <row r="10" spans="4:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D10" s="21" t="s">
+    <row r="9" spans="1:5" ht="5" customHeight="1">
+      <c r="A9" s="7"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="12"/>
+      <c r="E9" s="12"/>
+    </row>
+    <row r="10" spans="1:5" ht="19" customHeight="1">
+      <c r="A10" s="7"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="E10" s="21"/>
-    </row>
-    <row r="11" spans="4:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="D11" s="22" t="s">
+      <c r="E10" s="13"/>
+    </row>
+    <row r="11" spans="1:5" ht="13">
+      <c r="A11" s="7"/>
+      <c r="B11" s="8"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E11" s="22"/>
-    </row>
-    <row r="12" spans="4:5" ht="5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="E12" s="5"/>
-    </row>
-    <row r="13" spans="4:5" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D13" s="21" t="s">
+      <c r="E11" s="4"/>
+    </row>
+    <row r="12" spans="1:5" ht="5" customHeight="1">
+      <c r="A12" s="7"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="3"/>
+    </row>
+    <row r="13" spans="1:5" ht="18" customHeight="1">
+      <c r="A13" s="7"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="E13" s="21"/>
-    </row>
-    <row r="14" spans="4:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="D14" s="22" t="s">
+      <c r="E13" s="13"/>
+    </row>
+    <row r="14" spans="1:5" ht="13">
+      <c r="A14" s="7"/>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E14" s="22"/>
-    </row>
-    <row r="15" spans="4:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-    </row>
-    <row r="16" spans="4:5" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-    </row>
-    <row r="17" spans="1:5" ht="19" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D17" s="9" t="s">
+      <c r="E14" s="4"/>
+    </row>
+    <row r="15" spans="1:5" ht="13">
+      <c r="A15" s="7"/>
+      <c r="B15" s="8"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+    </row>
+    <row r="16" spans="1:5" ht="18" customHeight="1">
+      <c r="A16" s="7"/>
+      <c r="B16" s="8"/>
+      <c r="C16" s="8"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="14"/>
+    </row>
+    <row r="17" spans="1:5" ht="19" customHeight="1">
+      <c r="A17" s="7"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="15" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" ht="18" x14ac:dyDescent="0.15">
-      <c r="A20" s="17" t="s">
+      <c r="E17" s="8"/>
+    </row>
+    <row r="18" spans="1:5" ht="11.5" customHeight="1">
+      <c r="A18" s="7"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
+      <c r="D18" s="8"/>
+      <c r="E18" s="8"/>
+    </row>
+    <row r="19" spans="1:5" ht="11.5" customHeight="1">
+      <c r="A19" s="7"/>
+      <c r="B19" s="8"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+    </row>
+    <row r="20" spans="1:5" ht="13">
+      <c r="A20" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="B20" s="17"/>
-      <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-    </row>
-    <row r="21" spans="1:5" ht="8" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="22" spans="1:5" ht="8" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="23" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="32" t="s">
+      <c r="B20" s="16"/>
+      <c r="C20" s="16"/>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
+    </row>
+    <row r="21" spans="1:5" ht="8" customHeight="1">
+      <c r="A21" s="7"/>
+      <c r="B21" s="8"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+    </row>
+    <row r="22" spans="1:5" ht="8" customHeight="1">
+      <c r="A22" s="7"/>
+      <c r="B22" s="8"/>
+      <c r="C22" s="8"/>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+    </row>
+    <row r="23" spans="1:5" ht="41" customHeight="1">
+      <c r="A23" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B23" s="23" t="s">
+      <c r="B23" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="C23" s="23"/>
-      <c r="D23" s="23"/>
-      <c r="E23" s="23"/>
-    </row>
-    <row r="24" spans="1:5" ht="8" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="25" spans="1:5" ht="38" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="32" t="s">
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+    </row>
+    <row r="24" spans="1:5" ht="8" customHeight="1">
+      <c r="A24" s="7"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="8"/>
+      <c r="D24" s="8"/>
+      <c r="E24" s="8"/>
+    </row>
+    <row r="25" spans="1:5" ht="38" customHeight="1">
+      <c r="A25" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B25" s="23" t="s">
+      <c r="B25" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="C25" s="23"/>
-      <c r="D25" s="23"/>
-      <c r="E25" s="23"/>
-    </row>
-    <row r="26" spans="1:5" ht="8" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="27" spans="1:5" ht="39" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="32" t="s">
+      <c r="C25" s="17"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="17"/>
+    </row>
+    <row r="26" spans="1:5" ht="8" customHeight="1">
+      <c r="A26" s="7"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
+      <c r="D26" s="8"/>
+      <c r="E26" s="8"/>
+    </row>
+    <row r="27" spans="1:5" ht="39" customHeight="1">
+      <c r="A27" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B27" s="23" t="s">
+      <c r="B27" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="C27" s="23"/>
-      <c r="D27" s="23"/>
-      <c r="E27" s="23"/>
-    </row>
-    <row r="28" spans="1:5" ht="8" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="29" spans="1:5" ht="40" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A29" s="32" t="s">
+      <c r="C27" s="17"/>
+      <c r="D27" s="17"/>
+      <c r="E27" s="17"/>
+    </row>
+    <row r="28" spans="1:5" ht="8" customHeight="1">
+      <c r="A28" s="7"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="8"/>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
+    </row>
+    <row r="29" spans="1:5" ht="40" customHeight="1">
+      <c r="A29" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B29" s="17" t="s">
+      <c r="B29" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="C29" s="17"/>
-      <c r="D29" s="17"/>
-      <c r="E29" s="17"/>
-    </row>
-    <row r="30" spans="1:5" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A30" s="24" t="s">
+      <c r="C29" s="16"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="16"/>
+    </row>
+    <row r="30" spans="1:5" ht="13" customHeight="1">
+      <c r="A30" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="B30" s="24"/>
-      <c r="C30" s="24"/>
-      <c r="D30" s="24"/>
-      <c r="E30" s="24"/>
-    </row>
-    <row r="31" spans="1:5" ht="22" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B31" s="10" t="s">
+      <c r="B30" s="18"/>
+      <c r="C30" s="18"/>
+      <c r="D30" s="18"/>
+      <c r="E30" s="18"/>
+    </row>
+    <row r="31" spans="1:5" ht="22" customHeight="1">
+      <c r="A31" s="7"/>
+      <c r="B31" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="C31" s="17" t="s">
+      <c r="C31" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="D31" s="17"/>
-      <c r="E31" s="17"/>
-    </row>
-    <row r="32" spans="1:5" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B32" s="10"/>
-      <c r="C32" s="24" t="s">
+      <c r="D31" s="16"/>
+      <c r="E31" s="16"/>
+    </row>
+    <row r="32" spans="1:5" ht="13" customHeight="1">
+      <c r="A32" s="7"/>
+      <c r="B32" s="19"/>
+      <c r="C32" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="D32" s="24"/>
-      <c r="E32" s="24"/>
-    </row>
-    <row r="33" spans="1:5" s="4" customFormat="1" ht="18" x14ac:dyDescent="0.15">
-      <c r="B33" s="11"/>
-      <c r="C33" s="11"/>
-      <c r="D33" s="11"/>
-      <c r="E33" s="11"/>
-    </row>
-    <row r="34" spans="1:5" ht="29" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A34" s="27" t="s">
+      <c r="D32" s="18"/>
+      <c r="E32" s="18"/>
+    </row>
+    <row r="33" spans="1:5" s="2" customFormat="1" ht="13">
+      <c r="A33" s="8"/>
+      <c r="B33" s="20"/>
+      <c r="C33" s="20"/>
+      <c r="D33" s="20"/>
+      <c r="E33" s="20"/>
+    </row>
+    <row r="34" spans="1:5" ht="29" customHeight="1">
+      <c r="A34" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="B34" s="27"/>
-      <c r="C34" s="28" t="s">
+      <c r="B34" s="21"/>
+      <c r="C34" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D34" s="29"/>
-      <c r="E34" s="30" t="s">
+      <c r="D34" s="20"/>
+      <c r="E34" s="22" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="18" x14ac:dyDescent="0.2">
-      <c r="A35" s="24" t="s">
+    <row r="35" spans="1:5" ht="13">
+      <c r="A35" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="B35" s="24"/>
-      <c r="C35" s="13" t="s">
+      <c r="B35" s="18"/>
+      <c r="C35" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="E35" s="12"/>
-    </row>
-    <row r="38" spans="1:5" ht="16" x14ac:dyDescent="0.15">
-      <c r="A38" s="25" t="s">
+      <c r="D35" s="8"/>
+      <c r="E35" s="23"/>
+    </row>
+    <row r="36" spans="1:5" ht="11.5" customHeight="1">
+      <c r="A36" s="7"/>
+      <c r="B36" s="8"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="8"/>
+      <c r="E36" s="8"/>
+    </row>
+    <row r="37" spans="1:5" ht="11.5" customHeight="1">
+      <c r="A37" s="7"/>
+      <c r="B37" s="8"/>
+      <c r="C37" s="8"/>
+      <c r="D37" s="8"/>
+      <c r="E37" s="8"/>
+    </row>
+    <row r="38" spans="1:5" ht="13">
+      <c r="A38" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="B38" s="25"/>
-      <c r="C38" s="25"/>
-      <c r="D38" s="29"/>
-      <c r="E38" s="29"/>
-    </row>
-    <row r="39" spans="1:5" ht="18" x14ac:dyDescent="0.15">
-      <c r="A39" s="26" t="s">
+      <c r="B38" s="24"/>
+      <c r="C38" s="24"/>
+      <c r="D38" s="20"/>
+      <c r="E38" s="20"/>
+    </row>
+    <row r="39" spans="1:5" ht="13">
+      <c r="A39" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="B39" s="26"/>
-      <c r="C39" s="26"/>
-      <c r="D39" s="29"/>
-      <c r="E39" s="29"/>
-    </row>
-    <row r="40" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A40" s="16" t="s">
+      <c r="B39" s="24"/>
+      <c r="C39" s="24"/>
+      <c r="D39" s="20"/>
+      <c r="E39" s="20"/>
+    </row>
+    <row r="40" spans="1:5" ht="18" customHeight="1">
+      <c r="A40" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B40" s="16"/>
-      <c r="C40" s="16"/>
-      <c r="D40" s="29"/>
-      <c r="E40" s="14" t="s">
+      <c r="B40" s="5"/>
+      <c r="C40" s="5"/>
+      <c r="D40" s="20"/>
+      <c r="E40" s="25" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A41" s="19" t="s">
+    <row r="41" spans="1:5" ht="13" customHeight="1">
+      <c r="A41" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B41" s="19"/>
-      <c r="C41" s="19"/>
-      <c r="D41" s="29"/>
-      <c r="E41" s="7" t="s">
+      <c r="B41" s="5"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="20"/>
+      <c r="E41" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="11.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A42" s="31"/>
-      <c r="B42" s="29"/>
-      <c r="C42" s="29"/>
-      <c r="D42" s="29"/>
-      <c r="E42" s="29"/>
-    </row>
-    <row r="43" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A43" s="16" t="s">
+    <row r="42" spans="1:5" ht="11.5" customHeight="1">
+      <c r="A42" s="26"/>
+      <c r="B42" s="20"/>
+      <c r="C42" s="20"/>
+      <c r="D42" s="20"/>
+      <c r="E42" s="20"/>
+    </row>
+    <row r="43" spans="1:5" ht="18" customHeight="1">
+      <c r="A43" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="16"/>
-      <c r="C43" s="16"/>
-      <c r="D43" s="29"/>
-      <c r="E43" s="14"/>
-    </row>
-    <row r="44" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A44" s="19" t="s">
+      <c r="B43" s="5"/>
+      <c r="C43" s="5"/>
+      <c r="D43" s="20"/>
+      <c r="E43" s="25"/>
+    </row>
+    <row r="44" spans="1:5" ht="14">
+      <c r="A44" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B44" s="19"/>
-      <c r="C44" s="19"/>
-      <c r="D44" s="29"/>
-      <c r="E44" s="7" t="s">
+      <c r="B44" s="5"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="20"/>
+      <c r="E44" s="3" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A45" s="31"/>
-      <c r="B45" s="29"/>
-      <c r="C45" s="29"/>
-      <c r="D45" s="29"/>
-      <c r="E45" s="29"/>
-    </row>
-    <row r="46" spans="1:5" ht="18" x14ac:dyDescent="0.15">
-      <c r="A46" s="26" t="s">
+    <row r="45" spans="1:5" ht="18" customHeight="1">
+      <c r="A45" s="26"/>
+      <c r="B45" s="20"/>
+      <c r="C45" s="20"/>
+      <c r="D45" s="20"/>
+      <c r="E45" s="20"/>
+    </row>
+    <row r="46" spans="1:5" ht="13">
+      <c r="A46" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B46" s="26"/>
-      <c r="C46" s="26"/>
-      <c r="D46" s="29"/>
-      <c r="E46" s="29"/>
-    </row>
-    <row r="47" spans="1:5" ht="18" x14ac:dyDescent="0.15">
-      <c r="A47" s="31"/>
-      <c r="B47" s="18"/>
-      <c r="C47" s="18"/>
-      <c r="D47" s="29"/>
-      <c r="E47" s="14"/>
-    </row>
-    <row r="48" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A48" s="31"/>
-      <c r="B48" s="15" t="s">
+      <c r="B46" s="24"/>
+      <c r="C46" s="24"/>
+      <c r="D46" s="20"/>
+      <c r="E46" s="20"/>
+    </row>
+    <row r="47" spans="1:5" ht="13">
+      <c r="A47" s="26"/>
+      <c r="B47" s="27"/>
+      <c r="C47" s="27"/>
+      <c r="D47" s="20"/>
+      <c r="E47" s="25"/>
+    </row>
+    <row r="48" spans="1:5" ht="14">
+      <c r="A48" s="26"/>
+      <c r="B48" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C48" s="15"/>
-      <c r="D48" s="29"/>
-      <c r="E48" s="7" t="s">
+      <c r="C48" s="6"/>
+      <c r="D48" s="20"/>
+      <c r="E48" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="49" spans="1:5" ht="11.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A49" s="31"/>
-      <c r="B49" s="29"/>
-      <c r="C49" s="29"/>
-      <c r="D49" s="29"/>
-      <c r="E49" s="29"/>
-    </row>
-    <row r="50" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A50" s="16" t="s">
+    <row r="49" spans="1:5" ht="11.5" customHeight="1">
+      <c r="A49" s="26"/>
+      <c r="B49" s="20"/>
+      <c r="C49" s="20"/>
+      <c r="D49" s="20"/>
+      <c r="E49" s="20"/>
+    </row>
+    <row r="50" spans="1:5" ht="18" customHeight="1">
+      <c r="A50" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B50" s="16"/>
-      <c r="C50" s="16"/>
-      <c r="D50" s="29"/>
-      <c r="E50" s="14"/>
-    </row>
-    <row r="51" spans="1:5" ht="13" x14ac:dyDescent="0.15">
-      <c r="A51" s="19" t="s">
+      <c r="B50" s="5"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="20"/>
+      <c r="E50" s="25"/>
+    </row>
+    <row r="51" spans="1:5" ht="14">
+      <c r="A51" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="B51" s="19"/>
-      <c r="C51" s="19"/>
-      <c r="D51" s="29"/>
-      <c r="E51" s="7" t="s">
+      <c r="B51" s="5"/>
+      <c r="C51" s="5"/>
+      <c r="D51" s="20"/>
+      <c r="E51" s="3" t="s">
         <v>8</v>
       </c>
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <mergeCells count="27">
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="A20:E20"/>
     <mergeCell ref="A51:C51"/>
     <mergeCell ref="A30:E30"/>
     <mergeCell ref="C31:E31"/>
@@ -949,22 +1059,11 @@
     <mergeCell ref="A35:B35"/>
     <mergeCell ref="A38:C38"/>
     <mergeCell ref="A39:C39"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="B23:E23"/>
-    <mergeCell ref="B25:E25"/>
-    <mergeCell ref="B27:E27"/>
-    <mergeCell ref="B29:E29"/>
-    <mergeCell ref="A20:E20"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="D13:E13"/>
     <mergeCell ref="B48:C48"/>
     <mergeCell ref="B47:C47"/>
     <mergeCell ref="A50:C50"/>
   </mergeCells>
-  <phoneticPr fontId="5" type="noConversion"/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" scale="80" orientation="portrait"/>
 </worksheet>

</xml_diff>